<commit_message>
Mainly Revision Code (Mac)
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ankitsingh/Documents/GitHub/Python-Programs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997C1E97-1FFD-AB4B-928C-2B64EC9C0168}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74588CC6-F27A-854B-90C2-71815EAB17BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20500" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="483">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1474,6 +1474,12 @@
   </si>
   <si>
     <t>Was done in one go but space optimization is remaining(scheduled)</t>
+  </si>
+  <si>
+    <t>FlipBits</t>
+  </si>
+  <si>
+    <t>Maximum subarray sum after K concatenation</t>
   </si>
 </sst>
 </file>
@@ -1972,10 +1978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:F571"/>
+  <dimension ref="A1:F572"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A400" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I420" sqref="I420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2398,9 +2404,13 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
+      <c r="A46" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="C46" s="17"/>
     </row>
     <row r="47" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
@@ -6116,27 +6126,29 @@
       <c r="C474" s="11"/>
     </row>
     <row r="475" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="B475" s="7"/>
+      <c r="A475" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B475" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="C475" s="11"/>
     </row>
     <row r="476" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A476" s="8"/>
-      <c r="B476" s="7"/>
+      <c r="A476" s="5"/>
+      <c r="B476" s="6"/>
+      <c r="C476" s="6"/>
     </row>
     <row r="477" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A477" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="B477" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="C477" s="11"/>
+      <c r="A477" s="8"/>
+      <c r="B477" s="7"/>
     </row>
     <row r="478" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A478" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B478" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C478" s="11"/>
     </row>
@@ -6145,7 +6157,7 @@
         <v>452</v>
       </c>
       <c r="B479" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C479" s="11"/>
     </row>
@@ -6154,7 +6166,7 @@
         <v>452</v>
       </c>
       <c r="B480" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C480" s="11"/>
     </row>
@@ -6163,7 +6175,7 @@
         <v>452</v>
       </c>
       <c r="B481" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C481" s="11"/>
     </row>
@@ -6172,7 +6184,7 @@
         <v>452</v>
       </c>
       <c r="B482" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C482" s="11"/>
     </row>
@@ -6181,7 +6193,7 @@
         <v>452</v>
       </c>
       <c r="B483" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C483" s="11"/>
     </row>
@@ -6190,7 +6202,7 @@
         <v>452</v>
       </c>
       <c r="B484" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C484" s="11"/>
     </row>
@@ -6199,7 +6211,7 @@
         <v>452</v>
       </c>
       <c r="B485" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C485" s="11"/>
     </row>
@@ -6208,15 +6220,21 @@
         <v>452</v>
       </c>
       <c r="B486" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="C486" s="11"/>
+    </row>
+    <row r="487" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A487" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B487" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="C486" s="11"/>
-    </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C487" s="12"/>
-    </row>
-    <row r="502" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C502" s="4"/>
+      <c r="C487" s="11"/>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C488" s="12"/>
     </row>
     <row r="503" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C503" s="4"/>
@@ -6424,6 +6442,9 @@
     </row>
     <row r="571" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C571" s="4"/>
+    </row>
+    <row r="572" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C572" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6861,16 +6882,16 @@
     <hyperlink ref="B470" r:id="rId432" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
     <hyperlink ref="B469" r:id="rId433" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
     <hyperlink ref="B468" r:id="rId434" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B477" r:id="rId435" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B478" r:id="rId436" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B479" r:id="rId437" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B480" r:id="rId438" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B481" r:id="rId439" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B482" r:id="rId440" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B483" r:id="rId441" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B486" r:id="rId442" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B484" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B485" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B478" r:id="rId435" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B479" r:id="rId436" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B480" r:id="rId437" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B481" r:id="rId438" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B482" r:id="rId439" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B483" r:id="rId440" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B484" r:id="rId441" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B487" r:id="rId442" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B485" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B486" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="B360" r:id="rId445" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="B2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
     <hyperlink ref="B433" r:id="rId447" xr:uid="{61650621-1868-8E4A-8524-F3C28E945BED}"/>
@@ -6879,6 +6900,8 @@
     <hyperlink ref="B25" r:id="rId450" xr:uid="{29F9D0A1-F725-A243-9BD6-1B0B749F7797}"/>
     <hyperlink ref="B21" r:id="rId451" xr:uid="{F3911F0D-A6A4-9F45-8FDA-CA35D11C8B49}"/>
     <hyperlink ref="B45" r:id="rId452" xr:uid="{264D1846-99AB-0146-94AE-3C4226478DAB}"/>
+    <hyperlink ref="B46" r:id="rId453" xr:uid="{7C631E14-3868-4945-8EFF-6BF0699C85F2}"/>
+    <hyperlink ref="B475" r:id="rId454" xr:uid="{7CBCA6A4-691C-E34A-8835-618E75D9F46D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added Binary search concepts MAC
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ankitsingh/Documents/GitHub/Python-Programs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0897FD0B-B8D5-B841-B79B-8BAFBB9E643B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A7B53F-8B10-314F-A28B-7A6EC7F09100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20500" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20500" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2005,8 +2005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B144" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3034,7 +3034,7 @@
       <c r="B116" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C116" s="20"/>
+      <c r="C116" s="17"/>
     </row>
     <row r="117" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">

</xml_diff>

<commit_message>
COMMIT FROM MAC (LINKED LIST)
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ankitsingh/Documents/GitHub/Python-Programs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44948D09-0E46-0F4D-9B96-F2ECECCDAD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1082F3-346A-7146-A89C-4FFFC2F8E2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20500" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="490">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1449,9 +1449,6 @@
     <t>accp in one go</t>
   </si>
   <si>
-    <t>not able to solve yet</t>
-  </si>
-  <si>
     <t>Non-overlapping Intervals</t>
   </si>
   <si>
@@ -1498,6 +1495,12 @@
   </si>
   <si>
     <t>??? Graph q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theory :  to be revised later </t>
+  </si>
+  <si>
+    <t>not attempted</t>
   </si>
 </sst>
 </file>
@@ -2011,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F580"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2080,7 +2083,7 @@
       <c r="C8" s="18"/>
       <c r="E8" s="11"/>
       <c r="F8" t="s">
-        <v>472</v>
+        <v>489</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -2202,11 +2205,11 @@
         <v>4</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -2241,7 +2244,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C25" s="17"/>
     </row>
@@ -2295,7 +2298,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C31" s="17"/>
     </row>
@@ -2376,7 +2379,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C40" s="17"/>
     </row>
@@ -2407,7 +2410,7 @@
       </c>
       <c r="C43" s="17"/>
       <c r="D43" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -2435,14 +2438,14 @@
       <c r="B46" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="20"/>
+      <c r="C46" s="17"/>
     </row>
     <row r="47" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C47" s="17"/>
     </row>
@@ -2451,20 +2454,20 @@
         <v>4</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="C48" s="20"/>
+        <v>476</v>
+      </c>
+      <c r="C48" s="19"/>
     </row>
     <row r="49" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>484</v>
-      </c>
-      <c r="C49" s="20"/>
+        <v>483</v>
+      </c>
+      <c r="C49" s="19"/>
       <c r="D49" s="15" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -2644,7 +2647,7 @@
         <v>52</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C71" s="17"/>
     </row>
@@ -2977,7 +2980,7 @@
         <v>52</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C108" s="17"/>
     </row>
@@ -3049,7 +3052,7 @@
       <c r="B117" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C117" s="20"/>
+      <c r="C117" s="17"/>
     </row>
     <row r="118" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
@@ -3069,7 +3072,7 @@
       </c>
       <c r="C119" s="20"/>
       <c r="D119" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3081,7 +3084,7 @@
       </c>
       <c r="C120" s="17"/>
       <c r="D120" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3091,9 +3094,9 @@
       <c r="B121" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C121" s="20"/>
+      <c r="C121" s="17"/>
       <c r="D121" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3103,9 +3106,9 @@
       <c r="B122" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C122" s="20"/>
+      <c r="C122" s="17"/>
       <c r="D122" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3117,7 +3120,7 @@
       </c>
       <c r="C123" s="20"/>
       <c r="D123" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3129,7 +3132,7 @@
       </c>
       <c r="C124" s="20"/>
       <c r="D124" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3139,9 +3142,9 @@
       <c r="B125" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C125" s="20"/>
+      <c r="C125" s="17"/>
       <c r="D125" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3151,9 +3154,9 @@
       <c r="B126" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C126" s="20"/>
+      <c r="C126" s="17"/>
       <c r="D126" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3165,7 +3168,7 @@
       </c>
       <c r="C127" s="20"/>
       <c r="D127" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3177,7 +3180,7 @@
       </c>
       <c r="C128" s="17"/>
       <c r="D128" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3198,7 +3201,7 @@
       </c>
       <c r="C130" s="19"/>
       <c r="D130" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3228,7 +3231,7 @@
       </c>
       <c r="C133" s="17"/>
       <c r="D133" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3245,11 +3248,11 @@
         <v>96</v>
       </c>
       <c r="B135" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="C135" s="17"/>
+      <c r="D135" t="s">
         <v>486</v>
-      </c>
-      <c r="C135" s="20"/>
-      <c r="D135" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3261,7 +3264,7 @@
       </c>
       <c r="C136" s="17"/>
       <c r="D136" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -3271,7 +3274,7 @@
       <c r="B137" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C137" s="19"/>
+      <c r="C137" s="17"/>
     </row>
     <row r="138" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
@@ -3298,7 +3301,7 @@
       <c r="B140" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C140" s="20"/>
+      <c r="C140" s="17"/>
     </row>
     <row r="141" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
@@ -3336,7 +3339,7 @@
       </c>
       <c r="C144" s="17"/>
     </row>
-    <row r="145" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>96</v>
       </c>
@@ -3345,7 +3348,7 @@
       </c>
       <c r="C145" s="20"/>
     </row>
-    <row r="146" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>96</v>
       </c>
@@ -3354,7 +3357,7 @@
       </c>
       <c r="C146" s="17"/>
     </row>
-    <row r="147" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>96</v>
       </c>
@@ -3363,28 +3366,31 @@
       </c>
       <c r="C147" s="20"/>
     </row>
-    <row r="148" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B148" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C148" s="20"/>
-    </row>
-    <row r="150" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="C148" s="19"/>
+      <c r="D148" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="B150" s="7"/>
     </row>
-    <row r="151" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
         <v>132</v>
       </c>
       <c r="B151" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C151" s="20"/>
-    </row>
-    <row r="152" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="C151" s="17"/>
+    </row>
+    <row r="152" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
         <v>132</v>
       </c>
@@ -3393,7 +3399,7 @@
       </c>
       <c r="C152" s="20"/>
     </row>
-    <row r="153" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
         <v>132</v>
       </c>
@@ -3402,7 +3408,7 @@
       </c>
       <c r="C153" s="20"/>
     </row>
-    <row r="154" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
         <v>132</v>
       </c>
@@ -3411,7 +3417,7 @@
       </c>
       <c r="C154" s="20"/>
     </row>
-    <row r="155" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A155" s="8" t="s">
         <v>132</v>
       </c>
@@ -3420,7 +3426,7 @@
       </c>
       <c r="C155" s="20"/>
     </row>
-    <row r="156" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
         <v>132</v>
       </c>
@@ -3429,7 +3435,7 @@
       </c>
       <c r="C156" s="20"/>
     </row>
-    <row r="157" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
         <v>132</v>
       </c>
@@ -3438,7 +3444,7 @@
       </c>
       <c r="C157" s="20"/>
     </row>
-    <row r="158" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
         <v>132</v>
       </c>
@@ -3447,7 +3453,7 @@
       </c>
       <c r="C158" s="20"/>
     </row>
-    <row r="159" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
         <v>132</v>
       </c>
@@ -3456,7 +3462,7 @@
       </c>
       <c r="C159" s="20"/>
     </row>
-    <row r="160" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
         <v>132</v>
       </c>
@@ -6272,7 +6278,7 @@
         <v>391</v>
       </c>
       <c r="B483" s="6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C483" s="20"/>
     </row>

</xml_diff>